<commit_message>
variable for changes in hh info added, data prep code changed
</commit_message>
<xml_diff>
--- a/Mincome/Results/Different regressions.xlsx
+++ b/Mincome/Results/Different regressions.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\WU\Projekte\mincome\Mincome\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9165"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Tabellenblatt1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -174,18 +182,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -195,7 +209,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -223,60 +237,69 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -466,26 +489,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.43"/>
-    <col customWidth="1" min="7" max="7" width="48.0"/>
-    <col customWidth="1" min="10" max="10" width="78.71"/>
-    <col customWidth="1" min="12" max="12" width="51.71"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48" customWidth="1"/>
+    <col min="10" max="10" width="78.7109375" customWidth="1"/>
+    <col min="12" max="12" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -533,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -544,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="6" t="s">
@@ -557,10 +585,10 @@
         <v>11</v>
       </c>
       <c r="I3" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -571,7 +599,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="6" t="s">
@@ -584,10 +612,10 @@
         <v>14</v>
       </c>
       <c r="I4" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -598,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="5">
-        <v>435.0</v>
+        <v>435</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="6" t="s">
@@ -611,10 +639,10 @@
         <v>11</v>
       </c>
       <c r="I5" s="6">
-        <v>435.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -625,7 +653,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="6">
-        <v>435.0</v>
+        <v>435</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
@@ -638,10 +666,10 @@
         <v>17</v>
       </c>
       <c r="I6" s="6">
-        <v>435.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -652,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="6">
-        <v>275.0</v>
+        <v>275</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="6" t="s">
@@ -665,10 +693,10 @@
         <v>11</v>
       </c>
       <c r="I7" s="6">
-        <v>275.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -679,7 +707,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="6">
-        <v>275.0</v>
+        <v>275</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="6" t="s">
@@ -692,10 +720,10 @@
         <v>19</v>
       </c>
       <c r="I8" s="6">
-        <v>275.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -706,7 +734,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="5" t="s">
@@ -719,10 +747,10 @@
         <v>16</v>
       </c>
       <c r="I9" s="5">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -733,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="5" t="s">
@@ -746,10 +774,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="5">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -760,7 +788,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="6" t="s">
@@ -773,10 +801,10 @@
         <v>11</v>
       </c>
       <c r="I11" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
@@ -787,7 +815,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="6" t="s">
@@ -800,10 +828,10 @@
         <v>11</v>
       </c>
       <c r="I12" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
@@ -814,7 +842,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="6" t="s">
@@ -827,10 +855,10 @@
         <v>11</v>
       </c>
       <c r="I13" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
@@ -841,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="6" t="s">
@@ -854,10 +882,10 @@
         <v>11</v>
       </c>
       <c r="I14" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -868,7 +896,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="6" t="s">
@@ -881,10 +909,10 @@
         <v>11</v>
       </c>
       <c r="I15" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
@@ -895,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="6" t="s">
@@ -908,10 +936,10 @@
         <v>11</v>
       </c>
       <c r="I16" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -922,7 +950,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="5" t="s">
@@ -935,10 +963,10 @@
         <v>10</v>
       </c>
       <c r="I17" s="5">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
@@ -949,7 +977,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="5" t="s">
@@ -962,10 +990,10 @@
         <v>16</v>
       </c>
       <c r="I18" s="5">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
@@ -976,7 +1004,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="6" t="s">
@@ -989,10 +1017,10 @@
         <v>31</v>
       </c>
       <c r="I19" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1031,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="5">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="6" t="s">
@@ -1016,10 +1044,10 @@
         <v>34</v>
       </c>
       <c r="I20" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1058,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="6" t="s">
@@ -1043,10 +1071,10 @@
         <v>36</v>
       </c>
       <c r="I21" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
@@ -1057,7 +1085,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="7" t="s">
@@ -1070,10 +1098,10 @@
         <v>37</v>
       </c>
       <c r="I22" s="7">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1112,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="7" t="s">
@@ -1097,10 +1125,10 @@
         <v>38</v>
       </c>
       <c r="I23" s="7">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1139,7 @@
         <v>39</v>
       </c>
       <c r="D24" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="7" t="s">
@@ -1124,10 +1152,10 @@
         <v>39</v>
       </c>
       <c r="I24" s="7">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>12</v>
       </c>
@@ -1138,7 +1166,7 @@
         <v>40</v>
       </c>
       <c r="D25" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="6" t="s">
@@ -1151,10 +1179,10 @@
         <v>41</v>
       </c>
       <c r="I25" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -1165,7 +1193,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="6" t="s">
@@ -1178,10 +1206,10 @@
         <v>31</v>
       </c>
       <c r="I26" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1220,7 @@
         <v>31</v>
       </c>
       <c r="D27" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="6" t="s">
@@ -1205,10 +1233,10 @@
         <v>31</v>
       </c>
       <c r="I27" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
@@ -1219,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="D28" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="6" t="s">
@@ -1232,10 +1260,10 @@
         <v>31</v>
       </c>
       <c r="I28" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>12</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>46</v>
       </c>
       <c r="D29" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="6" t="s">
@@ -1259,10 +1287,10 @@
         <v>46</v>
       </c>
       <c r="I29" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
@@ -1273,7 +1301,7 @@
         <v>48</v>
       </c>
       <c r="D30" s="6">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="6" t="s">
@@ -1286,10 +1314,10 @@
         <v>48</v>
       </c>
       <c r="I30" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -1305,10 +1333,10 @@
         <v>51</v>
       </c>
       <c r="I31" s="6">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1318,7 +1346,7 @@
       <c r="H32" s="9"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1329,2911 +1357,2912 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E34" s="11"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E35" s="11"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E36" s="11"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E37" s="11"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E38" s="11"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E39" s="11"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E40" s="11"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E41" s="11"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E42" s="11"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E43" s="11"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E44" s="11"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E45" s="11"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E46" s="11"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E47" s="11"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E48" s="11"/>
     </row>
-    <row r="49">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E49" s="11"/>
     </row>
-    <row r="50">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E50" s="11"/>
     </row>
-    <row r="51">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E51" s="11"/>
     </row>
-    <row r="52">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E52" s="11"/>
     </row>
-    <row r="53">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E53" s="11"/>
     </row>
-    <row r="54">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E54" s="11"/>
     </row>
-    <row r="55">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E55" s="11"/>
     </row>
-    <row r="56">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E56" s="11"/>
     </row>
-    <row r="57">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E57" s="11"/>
     </row>
-    <row r="58">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E58" s="11"/>
     </row>
-    <row r="59">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E59" s="11"/>
     </row>
-    <row r="60">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E60" s="11"/>
     </row>
-    <row r="61">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E61" s="11"/>
     </row>
-    <row r="62">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E62" s="11"/>
     </row>
-    <row r="63">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E63" s="11"/>
     </row>
-    <row r="64">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E64" s="11"/>
     </row>
-    <row r="65">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E65" s="11"/>
     </row>
-    <row r="66">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E66" s="11"/>
     </row>
-    <row r="67">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E67" s="11"/>
     </row>
-    <row r="68">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E68" s="11"/>
     </row>
-    <row r="69">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E69" s="11"/>
     </row>
-    <row r="70">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E70" s="11"/>
     </row>
-    <row r="71">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E71" s="11"/>
     </row>
-    <row r="72">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E72" s="11"/>
     </row>
-    <row r="73">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E73" s="11"/>
     </row>
-    <row r="74">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E74" s="11"/>
     </row>
-    <row r="75">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E75" s="11"/>
     </row>
-    <row r="76">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E76" s="11"/>
     </row>
-    <row r="77">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E77" s="11"/>
     </row>
-    <row r="78">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E78" s="11"/>
     </row>
-    <row r="79">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E79" s="11"/>
     </row>
-    <row r="80">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E80" s="11"/>
     </row>
-    <row r="81">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="11"/>
     </row>
-    <row r="82">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E82" s="11"/>
     </row>
-    <row r="83">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E83" s="11"/>
     </row>
-    <row r="84">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E84" s="11"/>
     </row>
-    <row r="85">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E85" s="11"/>
     </row>
-    <row r="86">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E86" s="11"/>
     </row>
-    <row r="87">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E87" s="11"/>
     </row>
-    <row r="88">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E88" s="11"/>
     </row>
-    <row r="89">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E89" s="11"/>
     </row>
-    <row r="90">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E90" s="11"/>
     </row>
-    <row r="91">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E91" s="11"/>
     </row>
-    <row r="92">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E92" s="11"/>
     </row>
-    <row r="93">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E93" s="11"/>
     </row>
-    <row r="94">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E94" s="11"/>
     </row>
-    <row r="95">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E95" s="11"/>
     </row>
-    <row r="96">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E96" s="11"/>
     </row>
-    <row r="97">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E97" s="11"/>
     </row>
-    <row r="98">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E98" s="11"/>
     </row>
-    <row r="99">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E99" s="11"/>
     </row>
-    <row r="100">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E100" s="11"/>
     </row>
-    <row r="101">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E101" s="11"/>
     </row>
-    <row r="102">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E102" s="11"/>
     </row>
-    <row r="103">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E103" s="11"/>
     </row>
-    <row r="104">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E104" s="11"/>
     </row>
-    <row r="105">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E105" s="11"/>
     </row>
-    <row r="106">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E106" s="11"/>
     </row>
-    <row r="107">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E107" s="11"/>
     </row>
-    <row r="108">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E108" s="11"/>
     </row>
-    <row r="109">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E109" s="11"/>
     </row>
-    <row r="110">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E110" s="11"/>
     </row>
-    <row r="111">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E111" s="11"/>
     </row>
-    <row r="112">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E112" s="11"/>
     </row>
-    <row r="113">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E113" s="11"/>
     </row>
-    <row r="114">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E114" s="11"/>
     </row>
-    <row r="115">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E115" s="11"/>
     </row>
-    <row r="116">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E116" s="11"/>
     </row>
-    <row r="117">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E117" s="11"/>
     </row>
-    <row r="118">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E118" s="11"/>
     </row>
-    <row r="119">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E119" s="11"/>
     </row>
-    <row r="120">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E120" s="11"/>
     </row>
-    <row r="121">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E121" s="11"/>
     </row>
-    <row r="122">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E122" s="11"/>
     </row>
-    <row r="123">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E123" s="11"/>
     </row>
-    <row r="124">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E124" s="11"/>
     </row>
-    <row r="125">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E125" s="11"/>
     </row>
-    <row r="126">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E126" s="11"/>
     </row>
-    <row r="127">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E127" s="11"/>
     </row>
-    <row r="128">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E128" s="11"/>
     </row>
-    <row r="129">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E129" s="11"/>
     </row>
-    <row r="130">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E130" s="11"/>
     </row>
-    <row r="131">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E131" s="11"/>
     </row>
-    <row r="132">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E132" s="11"/>
     </row>
-    <row r="133">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E133" s="11"/>
     </row>
-    <row r="134">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E134" s="11"/>
     </row>
-    <row r="135">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E135" s="11"/>
     </row>
-    <row r="136">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E136" s="11"/>
     </row>
-    <row r="137">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E137" s="11"/>
     </row>
-    <row r="138">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E138" s="11"/>
     </row>
-    <row r="139">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E139" s="11"/>
     </row>
-    <row r="140">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E140" s="11"/>
     </row>
-    <row r="141">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E141" s="11"/>
     </row>
-    <row r="142">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E142" s="11"/>
     </row>
-    <row r="143">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E143" s="11"/>
     </row>
-    <row r="144">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E144" s="11"/>
     </row>
-    <row r="145">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E145" s="11"/>
     </row>
-    <row r="146">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E146" s="11"/>
     </row>
-    <row r="147">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E147" s="11"/>
     </row>
-    <row r="148">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E148" s="11"/>
     </row>
-    <row r="149">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E149" s="11"/>
     </row>
-    <row r="150">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E150" s="11"/>
     </row>
-    <row r="151">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E151" s="11"/>
     </row>
-    <row r="152">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E152" s="11"/>
     </row>
-    <row r="153">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E153" s="11"/>
     </row>
-    <row r="154">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E154" s="11"/>
     </row>
-    <row r="155">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E155" s="11"/>
     </row>
-    <row r="156">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E156" s="11"/>
     </row>
-    <row r="157">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E157" s="11"/>
     </row>
-    <row r="158">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E158" s="11"/>
     </row>
-    <row r="159">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E159" s="11"/>
     </row>
-    <row r="160">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E160" s="11"/>
     </row>
-    <row r="161">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E161" s="11"/>
     </row>
-    <row r="162">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E162" s="11"/>
     </row>
-    <row r="163">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163" s="11"/>
     </row>
-    <row r="164">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E164" s="11"/>
     </row>
-    <row r="165">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E165" s="11"/>
     </row>
-    <row r="166">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E166" s="11"/>
     </row>
-    <row r="167">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E167" s="11"/>
     </row>
-    <row r="168">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E168" s="11"/>
     </row>
-    <row r="169">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E169" s="11"/>
     </row>
-    <row r="170">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E170" s="11"/>
     </row>
-    <row r="171">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E171" s="11"/>
     </row>
-    <row r="172">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E172" s="11"/>
     </row>
-    <row r="173">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E173" s="11"/>
     </row>
-    <row r="174">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E174" s="11"/>
     </row>
-    <row r="175">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E175" s="11"/>
     </row>
-    <row r="176">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E176" s="11"/>
     </row>
-    <row r="177">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E177" s="11"/>
     </row>
-    <row r="178">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E178" s="11"/>
     </row>
-    <row r="179">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E179" s="11"/>
     </row>
-    <row r="180">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E180" s="11"/>
     </row>
-    <row r="181">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E181" s="11"/>
     </row>
-    <row r="182">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E182" s="11"/>
     </row>
-    <row r="183">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E183" s="11"/>
     </row>
-    <row r="184">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E184" s="11"/>
     </row>
-    <row r="185">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E185" s="11"/>
     </row>
-    <row r="186">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E186" s="11"/>
     </row>
-    <row r="187">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E187" s="11"/>
     </row>
-    <row r="188">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E188" s="11"/>
     </row>
-    <row r="189">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E189" s="11"/>
     </row>
-    <row r="190">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E190" s="11"/>
     </row>
-    <row r="191">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E191" s="11"/>
     </row>
-    <row r="192">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E192" s="11"/>
     </row>
-    <row r="193">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E193" s="11"/>
     </row>
-    <row r="194">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E194" s="11"/>
     </row>
-    <row r="195">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E195" s="11"/>
     </row>
-    <row r="196">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E196" s="11"/>
     </row>
-    <row r="197">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E197" s="11"/>
     </row>
-    <row r="198">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E198" s="11"/>
     </row>
-    <row r="199">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E199" s="11"/>
     </row>
-    <row r="200">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E200" s="11"/>
     </row>
-    <row r="201">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E201" s="11"/>
     </row>
-    <row r="202">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E202" s="11"/>
     </row>
-    <row r="203">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E203" s="11"/>
     </row>
-    <row r="204">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E204" s="11"/>
     </row>
-    <row r="205">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E205" s="11"/>
     </row>
-    <row r="206">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E206" s="11"/>
     </row>
-    <row r="207">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E207" s="11"/>
     </row>
-    <row r="208">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E208" s="11"/>
     </row>
-    <row r="209">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E209" s="11"/>
     </row>
-    <row r="210">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E210" s="11"/>
     </row>
-    <row r="211">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E211" s="11"/>
     </row>
-    <row r="212">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E212" s="11"/>
     </row>
-    <row r="213">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E213" s="11"/>
     </row>
-    <row r="214">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E214" s="11"/>
     </row>
-    <row r="215">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E215" s="11"/>
     </row>
-    <row r="216">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E216" s="11"/>
     </row>
-    <row r="217">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E217" s="11"/>
     </row>
-    <row r="218">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E218" s="11"/>
     </row>
-    <row r="219">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E219" s="11"/>
     </row>
-    <row r="220">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E220" s="11"/>
     </row>
-    <row r="221">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E221" s="11"/>
     </row>
-    <row r="222">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E222" s="11"/>
     </row>
-    <row r="223">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E223" s="11"/>
     </row>
-    <row r="224">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E224" s="11"/>
     </row>
-    <row r="225">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E225" s="11"/>
     </row>
-    <row r="226">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E226" s="11"/>
     </row>
-    <row r="227">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E227" s="11"/>
     </row>
-    <row r="228">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E228" s="11"/>
     </row>
-    <row r="229">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E229" s="11"/>
     </row>
-    <row r="230">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E230" s="11"/>
     </row>
-    <row r="231">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E231" s="11"/>
     </row>
-    <row r="232">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E232" s="11"/>
     </row>
-    <row r="233">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E233" s="11"/>
     </row>
-    <row r="234">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E234" s="11"/>
     </row>
-    <row r="235">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E235" s="11"/>
     </row>
-    <row r="236">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E236" s="11"/>
     </row>
-    <row r="237">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E237" s="11"/>
     </row>
-    <row r="238">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E238" s="11"/>
     </row>
-    <row r="239">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E239" s="11"/>
     </row>
-    <row r="240">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E240" s="11"/>
     </row>
-    <row r="241">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E241" s="11"/>
     </row>
-    <row r="242">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E242" s="11"/>
     </row>
-    <row r="243">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E243" s="11"/>
     </row>
-    <row r="244">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E244" s="11"/>
     </row>
-    <row r="245">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E245" s="11"/>
     </row>
-    <row r="246">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E246" s="11"/>
     </row>
-    <row r="247">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E247" s="11"/>
     </row>
-    <row r="248">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E248" s="11"/>
     </row>
-    <row r="249">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E249" s="11"/>
     </row>
-    <row r="250">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E250" s="11"/>
     </row>
-    <row r="251">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E251" s="11"/>
     </row>
-    <row r="252">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E252" s="11"/>
     </row>
-    <row r="253">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E253" s="11"/>
     </row>
-    <row r="254">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E254" s="11"/>
     </row>
-    <row r="255">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E255" s="11"/>
     </row>
-    <row r="256">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E256" s="11"/>
     </row>
-    <row r="257">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E257" s="11"/>
     </row>
-    <row r="258">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E258" s="11"/>
     </row>
-    <row r="259">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E259" s="11"/>
     </row>
-    <row r="260">
+    <row r="260" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E260" s="11"/>
     </row>
-    <row r="261">
+    <row r="261" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E261" s="11"/>
     </row>
-    <row r="262">
+    <row r="262" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E262" s="11"/>
     </row>
-    <row r="263">
+    <row r="263" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E263" s="11"/>
     </row>
-    <row r="264">
+    <row r="264" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E264" s="11"/>
     </row>
-    <row r="265">
+    <row r="265" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E265" s="11"/>
     </row>
-    <row r="266">
+    <row r="266" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E266" s="11"/>
     </row>
-    <row r="267">
+    <row r="267" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E267" s="11"/>
     </row>
-    <row r="268">
+    <row r="268" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E268" s="11"/>
     </row>
-    <row r="269">
+    <row r="269" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E269" s="11"/>
     </row>
-    <row r="270">
+    <row r="270" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E270" s="11"/>
     </row>
-    <row r="271">
+    <row r="271" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E271" s="11"/>
     </row>
-    <row r="272">
+    <row r="272" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E272" s="11"/>
     </row>
-    <row r="273">
+    <row r="273" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E273" s="11"/>
     </row>
-    <row r="274">
+    <row r="274" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E274" s="11"/>
     </row>
-    <row r="275">
+    <row r="275" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E275" s="11"/>
     </row>
-    <row r="276">
+    <row r="276" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E276" s="11"/>
     </row>
-    <row r="277">
+    <row r="277" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E277" s="11"/>
     </row>
-    <row r="278">
+    <row r="278" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E278" s="11"/>
     </row>
-    <row r="279">
+    <row r="279" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E279" s="11"/>
     </row>
-    <row r="280">
+    <row r="280" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E280" s="11"/>
     </row>
-    <row r="281">
+    <row r="281" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E281" s="11"/>
     </row>
-    <row r="282">
+    <row r="282" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E282" s="11"/>
     </row>
-    <row r="283">
+    <row r="283" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E283" s="11"/>
     </row>
-    <row r="284">
+    <row r="284" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E284" s="11"/>
     </row>
-    <row r="285">
+    <row r="285" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E285" s="11"/>
     </row>
-    <row r="286">
+    <row r="286" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E286" s="11"/>
     </row>
-    <row r="287">
+    <row r="287" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E287" s="11"/>
     </row>
-    <row r="288">
+    <row r="288" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E288" s="11"/>
     </row>
-    <row r="289">
+    <row r="289" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E289" s="11"/>
     </row>
-    <row r="290">
+    <row r="290" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E290" s="11"/>
     </row>
-    <row r="291">
+    <row r="291" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E291" s="11"/>
     </row>
-    <row r="292">
+    <row r="292" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E292" s="11"/>
     </row>
-    <row r="293">
+    <row r="293" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E293" s="11"/>
     </row>
-    <row r="294">
+    <row r="294" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E294" s="11"/>
     </row>
-    <row r="295">
+    <row r="295" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E295" s="11"/>
     </row>
-    <row r="296">
+    <row r="296" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E296" s="11"/>
     </row>
-    <row r="297">
+    <row r="297" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E297" s="11"/>
     </row>
-    <row r="298">
+    <row r="298" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E298" s="11"/>
     </row>
-    <row r="299">
+    <row r="299" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E299" s="11"/>
     </row>
-    <row r="300">
+    <row r="300" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E300" s="11"/>
     </row>
-    <row r="301">
+    <row r="301" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E301" s="11"/>
     </row>
-    <row r="302">
+    <row r="302" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E302" s="11"/>
     </row>
-    <row r="303">
+    <row r="303" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E303" s="11"/>
     </row>
-    <row r="304">
+    <row r="304" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E304" s="11"/>
     </row>
-    <row r="305">
+    <row r="305" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E305" s="11"/>
     </row>
-    <row r="306">
+    <row r="306" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E306" s="11"/>
     </row>
-    <row r="307">
+    <row r="307" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E307" s="11"/>
     </row>
-    <row r="308">
+    <row r="308" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E308" s="11"/>
     </row>
-    <row r="309">
+    <row r="309" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E309" s="11"/>
     </row>
-    <row r="310">
+    <row r="310" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E310" s="11"/>
     </row>
-    <row r="311">
+    <row r="311" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E311" s="11"/>
     </row>
-    <row r="312">
+    <row r="312" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E312" s="11"/>
     </row>
-    <row r="313">
+    <row r="313" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E313" s="11"/>
     </row>
-    <row r="314">
+    <row r="314" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E314" s="11"/>
     </row>
-    <row r="315">
+    <row r="315" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E315" s="11"/>
     </row>
-    <row r="316">
+    <row r="316" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E316" s="11"/>
     </row>
-    <row r="317">
+    <row r="317" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E317" s="11"/>
     </row>
-    <row r="318">
+    <row r="318" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E318" s="11"/>
     </row>
-    <row r="319">
+    <row r="319" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E319" s="11"/>
     </row>
-    <row r="320">
+    <row r="320" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E320" s="11"/>
     </row>
-    <row r="321">
+    <row r="321" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E321" s="11"/>
     </row>
-    <row r="322">
+    <row r="322" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E322" s="11"/>
     </row>
-    <row r="323">
+    <row r="323" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E323" s="11"/>
     </row>
-    <row r="324">
+    <row r="324" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E324" s="11"/>
     </row>
-    <row r="325">
+    <row r="325" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E325" s="11"/>
     </row>
-    <row r="326">
+    <row r="326" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E326" s="11"/>
     </row>
-    <row r="327">
+    <row r="327" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E327" s="11"/>
     </row>
-    <row r="328">
+    <row r="328" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E328" s="11"/>
     </row>
-    <row r="329">
+    <row r="329" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E329" s="11"/>
     </row>
-    <row r="330">
+    <row r="330" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E330" s="11"/>
     </row>
-    <row r="331">
+    <row r="331" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E331" s="11"/>
     </row>
-    <row r="332">
+    <row r="332" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E332" s="11"/>
     </row>
-    <row r="333">
+    <row r="333" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E333" s="11"/>
     </row>
-    <row r="334">
+    <row r="334" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E334" s="11"/>
     </row>
-    <row r="335">
+    <row r="335" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E335" s="11"/>
     </row>
-    <row r="336">
+    <row r="336" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E336" s="11"/>
     </row>
-    <row r="337">
+    <row r="337" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E337" s="11"/>
     </row>
-    <row r="338">
+    <row r="338" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E338" s="11"/>
     </row>
-    <row r="339">
+    <row r="339" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E339" s="11"/>
     </row>
-    <row r="340">
+    <row r="340" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E340" s="11"/>
     </row>
-    <row r="341">
+    <row r="341" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E341" s="11"/>
     </row>
-    <row r="342">
+    <row r="342" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E342" s="11"/>
     </row>
-    <row r="343">
+    <row r="343" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E343" s="11"/>
     </row>
-    <row r="344">
+    <row r="344" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E344" s="11"/>
     </row>
-    <row r="345">
+    <row r="345" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E345" s="11"/>
     </row>
-    <row r="346">
+    <row r="346" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E346" s="11"/>
     </row>
-    <row r="347">
+    <row r="347" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E347" s="11"/>
     </row>
-    <row r="348">
+    <row r="348" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E348" s="11"/>
     </row>
-    <row r="349">
+    <row r="349" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E349" s="11"/>
     </row>
-    <row r="350">
+    <row r="350" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E350" s="11"/>
     </row>
-    <row r="351">
+    <row r="351" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E351" s="11"/>
     </row>
-    <row r="352">
+    <row r="352" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E352" s="11"/>
     </row>
-    <row r="353">
+    <row r="353" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E353" s="11"/>
     </row>
-    <row r="354">
+    <row r="354" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E354" s="11"/>
     </row>
-    <row r="355">
+    <row r="355" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E355" s="11"/>
     </row>
-    <row r="356">
+    <row r="356" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E356" s="11"/>
     </row>
-    <row r="357">
+    <row r="357" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E357" s="11"/>
     </row>
-    <row r="358">
+    <row r="358" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E358" s="11"/>
     </row>
-    <row r="359">
+    <row r="359" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E359" s="11"/>
     </row>
-    <row r="360">
+    <row r="360" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E360" s="11"/>
     </row>
-    <row r="361">
+    <row r="361" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E361" s="11"/>
     </row>
-    <row r="362">
+    <row r="362" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E362" s="11"/>
     </row>
-    <row r="363">
+    <row r="363" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E363" s="11"/>
     </row>
-    <row r="364">
+    <row r="364" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E364" s="11"/>
     </row>
-    <row r="365">
+    <row r="365" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E365" s="11"/>
     </row>
-    <row r="366">
+    <row r="366" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E366" s="11"/>
     </row>
-    <row r="367">
+    <row r="367" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E367" s="11"/>
     </row>
-    <row r="368">
+    <row r="368" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E368" s="11"/>
     </row>
-    <row r="369">
+    <row r="369" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E369" s="11"/>
     </row>
-    <row r="370">
+    <row r="370" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E370" s="11"/>
     </row>
-    <row r="371">
+    <row r="371" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E371" s="11"/>
     </row>
-    <row r="372">
+    <row r="372" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E372" s="11"/>
     </row>
-    <row r="373">
+    <row r="373" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E373" s="11"/>
     </row>
-    <row r="374">
+    <row r="374" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E374" s="11"/>
     </row>
-    <row r="375">
+    <row r="375" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E375" s="11"/>
     </row>
-    <row r="376">
+    <row r="376" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E376" s="11"/>
     </row>
-    <row r="377">
+    <row r="377" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E377" s="11"/>
     </row>
-    <row r="378">
+    <row r="378" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E378" s="11"/>
     </row>
-    <row r="379">
+    <row r="379" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E379" s="11"/>
     </row>
-    <row r="380">
+    <row r="380" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E380" s="11"/>
     </row>
-    <row r="381">
+    <row r="381" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E381" s="11"/>
     </row>
-    <row r="382">
+    <row r="382" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E382" s="11"/>
     </row>
-    <row r="383">
+    <row r="383" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E383" s="11"/>
     </row>
-    <row r="384">
+    <row r="384" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E384" s="11"/>
     </row>
-    <row r="385">
+    <row r="385" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E385" s="11"/>
     </row>
-    <row r="386">
+    <row r="386" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E386" s="11"/>
     </row>
-    <row r="387">
+    <row r="387" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E387" s="11"/>
     </row>
-    <row r="388">
+    <row r="388" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E388" s="11"/>
     </row>
-    <row r="389">
+    <row r="389" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E389" s="11"/>
     </row>
-    <row r="390">
+    <row r="390" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E390" s="11"/>
     </row>
-    <row r="391">
+    <row r="391" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E391" s="11"/>
     </row>
-    <row r="392">
+    <row r="392" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E392" s="11"/>
     </row>
-    <row r="393">
+    <row r="393" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E393" s="11"/>
     </row>
-    <row r="394">
+    <row r="394" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E394" s="11"/>
     </row>
-    <row r="395">
+    <row r="395" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E395" s="11"/>
     </row>
-    <row r="396">
+    <row r="396" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E396" s="11"/>
     </row>
-    <row r="397">
+    <row r="397" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E397" s="11"/>
     </row>
-    <row r="398">
+    <row r="398" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E398" s="11"/>
     </row>
-    <row r="399">
+    <row r="399" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E399" s="11"/>
     </row>
-    <row r="400">
+    <row r="400" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E400" s="11"/>
     </row>
-    <row r="401">
+    <row r="401" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E401" s="11"/>
     </row>
-    <row r="402">
+    <row r="402" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E402" s="11"/>
     </row>
-    <row r="403">
+    <row r="403" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E403" s="11"/>
     </row>
-    <row r="404">
+    <row r="404" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E404" s="11"/>
     </row>
-    <row r="405">
+    <row r="405" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E405" s="11"/>
     </row>
-    <row r="406">
+    <row r="406" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E406" s="11"/>
     </row>
-    <row r="407">
+    <row r="407" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E407" s="11"/>
     </row>
-    <row r="408">
+    <row r="408" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E408" s="11"/>
     </row>
-    <row r="409">
+    <row r="409" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E409" s="11"/>
     </row>
-    <row r="410">
+    <row r="410" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E410" s="11"/>
     </row>
-    <row r="411">
+    <row r="411" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E411" s="11"/>
     </row>
-    <row r="412">
+    <row r="412" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E412" s="11"/>
     </row>
-    <row r="413">
+    <row r="413" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E413" s="11"/>
     </row>
-    <row r="414">
+    <row r="414" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E414" s="11"/>
     </row>
-    <row r="415">
+    <row r="415" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E415" s="11"/>
     </row>
-    <row r="416">
+    <row r="416" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E416" s="11"/>
     </row>
-    <row r="417">
+    <row r="417" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E417" s="11"/>
     </row>
-    <row r="418">
+    <row r="418" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E418" s="11"/>
     </row>
-    <row r="419">
+    <row r="419" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E419" s="11"/>
     </row>
-    <row r="420">
+    <row r="420" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E420" s="11"/>
     </row>
-    <row r="421">
+    <row r="421" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E421" s="11"/>
     </row>
-    <row r="422">
+    <row r="422" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E422" s="11"/>
     </row>
-    <row r="423">
+    <row r="423" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E423" s="11"/>
     </row>
-    <row r="424">
+    <row r="424" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E424" s="11"/>
     </row>
-    <row r="425">
+    <row r="425" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E425" s="11"/>
     </row>
-    <row r="426">
+    <row r="426" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E426" s="11"/>
     </row>
-    <row r="427">
+    <row r="427" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E427" s="11"/>
     </row>
-    <row r="428">
+    <row r="428" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E428" s="11"/>
     </row>
-    <row r="429">
+    <row r="429" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E429" s="11"/>
     </row>
-    <row r="430">
+    <row r="430" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E430" s="11"/>
     </row>
-    <row r="431">
+    <row r="431" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E431" s="11"/>
     </row>
-    <row r="432">
+    <row r="432" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E432" s="11"/>
     </row>
-    <row r="433">
+    <row r="433" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E433" s="11"/>
     </row>
-    <row r="434">
+    <row r="434" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E434" s="11"/>
     </row>
-    <row r="435">
+    <row r="435" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E435" s="11"/>
     </row>
-    <row r="436">
+    <row r="436" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E436" s="11"/>
     </row>
-    <row r="437">
+    <row r="437" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E437" s="11"/>
     </row>
-    <row r="438">
+    <row r="438" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E438" s="11"/>
     </row>
-    <row r="439">
+    <row r="439" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E439" s="11"/>
     </row>
-    <row r="440">
+    <row r="440" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E440" s="11"/>
     </row>
-    <row r="441">
+    <row r="441" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E441" s="11"/>
     </row>
-    <row r="442">
+    <row r="442" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E442" s="11"/>
     </row>
-    <row r="443">
+    <row r="443" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E443" s="11"/>
     </row>
-    <row r="444">
+    <row r="444" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E444" s="11"/>
     </row>
-    <row r="445">
+    <row r="445" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E445" s="11"/>
     </row>
-    <row r="446">
+    <row r="446" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E446" s="11"/>
     </row>
-    <row r="447">
+    <row r="447" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E447" s="11"/>
     </row>
-    <row r="448">
+    <row r="448" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E448" s="11"/>
     </row>
-    <row r="449">
+    <row r="449" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E449" s="11"/>
     </row>
-    <row r="450">
+    <row r="450" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E450" s="11"/>
     </row>
-    <row r="451">
+    <row r="451" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E451" s="11"/>
     </row>
-    <row r="452">
+    <row r="452" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E452" s="11"/>
     </row>
-    <row r="453">
+    <row r="453" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E453" s="11"/>
     </row>
-    <row r="454">
+    <row r="454" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E454" s="11"/>
     </row>
-    <row r="455">
+    <row r="455" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E455" s="11"/>
     </row>
-    <row r="456">
+    <row r="456" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E456" s="11"/>
     </row>
-    <row r="457">
+    <row r="457" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E457" s="11"/>
     </row>
-    <row r="458">
+    <row r="458" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E458" s="11"/>
     </row>
-    <row r="459">
+    <row r="459" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E459" s="11"/>
     </row>
-    <row r="460">
+    <row r="460" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E460" s="11"/>
     </row>
-    <row r="461">
+    <row r="461" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E461" s="11"/>
     </row>
-    <row r="462">
+    <row r="462" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E462" s="11"/>
     </row>
-    <row r="463">
+    <row r="463" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E463" s="11"/>
     </row>
-    <row r="464">
+    <row r="464" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E464" s="11"/>
     </row>
-    <row r="465">
+    <row r="465" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E465" s="11"/>
     </row>
-    <row r="466">
+    <row r="466" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E466" s="11"/>
     </row>
-    <row r="467">
+    <row r="467" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E467" s="11"/>
     </row>
-    <row r="468">
+    <row r="468" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E468" s="11"/>
     </row>
-    <row r="469">
+    <row r="469" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E469" s="11"/>
     </row>
-    <row r="470">
+    <row r="470" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E470" s="11"/>
     </row>
-    <row r="471">
+    <row r="471" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E471" s="11"/>
     </row>
-    <row r="472">
+    <row r="472" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E472" s="11"/>
     </row>
-    <row r="473">
+    <row r="473" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E473" s="11"/>
     </row>
-    <row r="474">
+    <row r="474" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E474" s="11"/>
     </row>
-    <row r="475">
+    <row r="475" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E475" s="11"/>
     </row>
-    <row r="476">
+    <row r="476" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E476" s="11"/>
     </row>
-    <row r="477">
+    <row r="477" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E477" s="11"/>
     </row>
-    <row r="478">
+    <row r="478" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E478" s="11"/>
     </row>
-    <row r="479">
+    <row r="479" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E479" s="11"/>
     </row>
-    <row r="480">
+    <row r="480" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E480" s="11"/>
     </row>
-    <row r="481">
+    <row r="481" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E481" s="11"/>
     </row>
-    <row r="482">
+    <row r="482" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E482" s="11"/>
     </row>
-    <row r="483">
+    <row r="483" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E483" s="11"/>
     </row>
-    <row r="484">
+    <row r="484" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E484" s="11"/>
     </row>
-    <row r="485">
+    <row r="485" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E485" s="11"/>
     </row>
-    <row r="486">
+    <row r="486" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E486" s="11"/>
     </row>
-    <row r="487">
+    <row r="487" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E487" s="11"/>
     </row>
-    <row r="488">
+    <row r="488" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E488" s="11"/>
     </row>
-    <row r="489">
+    <row r="489" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E489" s="11"/>
     </row>
-    <row r="490">
+    <row r="490" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E490" s="11"/>
     </row>
-    <row r="491">
+    <row r="491" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E491" s="11"/>
     </row>
-    <row r="492">
+    <row r="492" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E492" s="11"/>
     </row>
-    <row r="493">
+    <row r="493" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E493" s="11"/>
     </row>
-    <row r="494">
+    <row r="494" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E494" s="11"/>
     </row>
-    <row r="495">
+    <row r="495" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E495" s="11"/>
     </row>
-    <row r="496">
+    <row r="496" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E496" s="11"/>
     </row>
-    <row r="497">
+    <row r="497" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E497" s="11"/>
     </row>
-    <row r="498">
+    <row r="498" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E498" s="11"/>
     </row>
-    <row r="499">
+    <row r="499" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E499" s="11"/>
     </row>
-    <row r="500">
+    <row r="500" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E500" s="11"/>
     </row>
-    <row r="501">
+    <row r="501" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E501" s="11"/>
     </row>
-    <row r="502">
+    <row r="502" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E502" s="11"/>
     </row>
-    <row r="503">
+    <row r="503" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E503" s="11"/>
     </row>
-    <row r="504">
+    <row r="504" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E504" s="11"/>
     </row>
-    <row r="505">
+    <row r="505" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E505" s="11"/>
     </row>
-    <row r="506">
+    <row r="506" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E506" s="11"/>
     </row>
-    <row r="507">
+    <row r="507" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E507" s="11"/>
     </row>
-    <row r="508">
+    <row r="508" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E508" s="11"/>
     </row>
-    <row r="509">
+    <row r="509" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E509" s="11"/>
     </row>
-    <row r="510">
+    <row r="510" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E510" s="11"/>
     </row>
-    <row r="511">
+    <row r="511" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E511" s="11"/>
     </row>
-    <row r="512">
+    <row r="512" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E512" s="11"/>
     </row>
-    <row r="513">
+    <row r="513" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E513" s="11"/>
     </row>
-    <row r="514">
+    <row r="514" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E514" s="11"/>
     </row>
-    <row r="515">
+    <row r="515" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E515" s="11"/>
     </row>
-    <row r="516">
+    <row r="516" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E516" s="11"/>
     </row>
-    <row r="517">
+    <row r="517" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E517" s="11"/>
     </row>
-    <row r="518">
+    <row r="518" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E518" s="11"/>
     </row>
-    <row r="519">
+    <row r="519" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E519" s="11"/>
     </row>
-    <row r="520">
+    <row r="520" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E520" s="11"/>
     </row>
-    <row r="521">
+    <row r="521" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E521" s="11"/>
     </row>
-    <row r="522">
+    <row r="522" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E522" s="11"/>
     </row>
-    <row r="523">
+    <row r="523" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E523" s="11"/>
     </row>
-    <row r="524">
+    <row r="524" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E524" s="11"/>
     </row>
-    <row r="525">
+    <row r="525" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E525" s="11"/>
     </row>
-    <row r="526">
+    <row r="526" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E526" s="11"/>
     </row>
-    <row r="527">
+    <row r="527" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E527" s="11"/>
     </row>
-    <row r="528">
+    <row r="528" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E528" s="11"/>
     </row>
-    <row r="529">
+    <row r="529" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E529" s="11"/>
     </row>
-    <row r="530">
+    <row r="530" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E530" s="11"/>
     </row>
-    <row r="531">
+    <row r="531" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E531" s="11"/>
     </row>
-    <row r="532">
+    <row r="532" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E532" s="11"/>
     </row>
-    <row r="533">
+    <row r="533" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E533" s="11"/>
     </row>
-    <row r="534">
+    <row r="534" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E534" s="11"/>
     </row>
-    <row r="535">
+    <row r="535" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E535" s="11"/>
     </row>
-    <row r="536">
+    <row r="536" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E536" s="11"/>
     </row>
-    <row r="537">
+    <row r="537" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E537" s="11"/>
     </row>
-    <row r="538">
+    <row r="538" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E538" s="11"/>
     </row>
-    <row r="539">
+    <row r="539" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E539" s="11"/>
     </row>
-    <row r="540">
+    <row r="540" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E540" s="11"/>
     </row>
-    <row r="541">
+    <row r="541" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E541" s="11"/>
     </row>
-    <row r="542">
+    <row r="542" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E542" s="11"/>
     </row>
-    <row r="543">
+    <row r="543" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E543" s="11"/>
     </row>
-    <row r="544">
+    <row r="544" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E544" s="11"/>
     </row>
-    <row r="545">
+    <row r="545" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E545" s="11"/>
     </row>
-    <row r="546">
+    <row r="546" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E546" s="11"/>
     </row>
-    <row r="547">
+    <row r="547" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E547" s="11"/>
     </row>
-    <row r="548">
+    <row r="548" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E548" s="11"/>
     </row>
-    <row r="549">
+    <row r="549" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E549" s="11"/>
     </row>
-    <row r="550">
+    <row r="550" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E550" s="11"/>
     </row>
-    <row r="551">
+    <row r="551" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E551" s="11"/>
     </row>
-    <row r="552">
+    <row r="552" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E552" s="11"/>
     </row>
-    <row r="553">
+    <row r="553" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E553" s="11"/>
     </row>
-    <row r="554">
+    <row r="554" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E554" s="11"/>
     </row>
-    <row r="555">
+    <row r="555" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E555" s="11"/>
     </row>
-    <row r="556">
+    <row r="556" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E556" s="11"/>
     </row>
-    <row r="557">
+    <row r="557" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E557" s="11"/>
     </row>
-    <row r="558">
+    <row r="558" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E558" s="11"/>
     </row>
-    <row r="559">
+    <row r="559" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E559" s="11"/>
     </row>
-    <row r="560">
+    <row r="560" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E560" s="11"/>
     </row>
-    <row r="561">
+    <row r="561" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E561" s="11"/>
     </row>
-    <row r="562">
+    <row r="562" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E562" s="11"/>
     </row>
-    <row r="563">
+    <row r="563" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E563" s="11"/>
     </row>
-    <row r="564">
+    <row r="564" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E564" s="11"/>
     </row>
-    <row r="565">
+    <row r="565" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E565" s="11"/>
     </row>
-    <row r="566">
+    <row r="566" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E566" s="11"/>
     </row>
-    <row r="567">
+    <row r="567" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E567" s="11"/>
     </row>
-    <row r="568">
+    <row r="568" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E568" s="11"/>
     </row>
-    <row r="569">
+    <row r="569" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E569" s="11"/>
     </row>
-    <row r="570">
+    <row r="570" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E570" s="11"/>
     </row>
-    <row r="571">
+    <row r="571" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E571" s="11"/>
     </row>
-    <row r="572">
+    <row r="572" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E572" s="11"/>
     </row>
-    <row r="573">
+    <row r="573" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E573" s="11"/>
     </row>
-    <row r="574">
+    <row r="574" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E574" s="11"/>
     </row>
-    <row r="575">
+    <row r="575" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E575" s="11"/>
     </row>
-    <row r="576">
+    <row r="576" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E576" s="11"/>
     </row>
-    <row r="577">
+    <row r="577" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E577" s="11"/>
     </row>
-    <row r="578">
+    <row r="578" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E578" s="11"/>
     </row>
-    <row r="579">
+    <row r="579" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E579" s="11"/>
     </row>
-    <row r="580">
+    <row r="580" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E580" s="11"/>
     </row>
-    <row r="581">
+    <row r="581" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E581" s="11"/>
     </row>
-    <row r="582">
+    <row r="582" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E582" s="11"/>
     </row>
-    <row r="583">
+    <row r="583" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E583" s="11"/>
     </row>
-    <row r="584">
+    <row r="584" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E584" s="11"/>
     </row>
-    <row r="585">
+    <row r="585" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E585" s="11"/>
     </row>
-    <row r="586">
+    <row r="586" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E586" s="11"/>
     </row>
-    <row r="587">
+    <row r="587" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E587" s="11"/>
     </row>
-    <row r="588">
+    <row r="588" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E588" s="11"/>
     </row>
-    <row r="589">
+    <row r="589" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E589" s="11"/>
     </row>
-    <row r="590">
+    <row r="590" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E590" s="11"/>
     </row>
-    <row r="591">
+    <row r="591" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E591" s="11"/>
     </row>
-    <row r="592">
+    <row r="592" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E592" s="11"/>
     </row>
-    <row r="593">
+    <row r="593" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E593" s="11"/>
     </row>
-    <row r="594">
+    <row r="594" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E594" s="11"/>
     </row>
-    <row r="595">
+    <row r="595" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E595" s="11"/>
     </row>
-    <row r="596">
+    <row r="596" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E596" s="11"/>
     </row>
-    <row r="597">
+    <row r="597" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E597" s="11"/>
     </row>
-    <row r="598">
+    <row r="598" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E598" s="11"/>
     </row>
-    <row r="599">
+    <row r="599" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E599" s="11"/>
     </row>
-    <row r="600">
+    <row r="600" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E600" s="11"/>
     </row>
-    <row r="601">
+    <row r="601" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E601" s="11"/>
     </row>
-    <row r="602">
+    <row r="602" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E602" s="11"/>
     </row>
-    <row r="603">
+    <row r="603" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E603" s="11"/>
     </row>
-    <row r="604">
+    <row r="604" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E604" s="11"/>
     </row>
-    <row r="605">
+    <row r="605" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E605" s="11"/>
     </row>
-    <row r="606">
+    <row r="606" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E606" s="11"/>
     </row>
-    <row r="607">
+    <row r="607" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E607" s="11"/>
     </row>
-    <row r="608">
+    <row r="608" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E608" s="11"/>
     </row>
-    <row r="609">
+    <row r="609" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E609" s="11"/>
     </row>
-    <row r="610">
+    <row r="610" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E610" s="11"/>
     </row>
-    <row r="611">
+    <row r="611" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E611" s="11"/>
     </row>
-    <row r="612">
+    <row r="612" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E612" s="11"/>
     </row>
-    <row r="613">
+    <row r="613" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E613" s="11"/>
     </row>
-    <row r="614">
+    <row r="614" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E614" s="11"/>
     </row>
-    <row r="615">
+    <row r="615" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E615" s="11"/>
     </row>
-    <row r="616">
+    <row r="616" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E616" s="11"/>
     </row>
-    <row r="617">
+    <row r="617" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E617" s="11"/>
     </row>
-    <row r="618">
+    <row r="618" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E618" s="11"/>
     </row>
-    <row r="619">
+    <row r="619" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E619" s="11"/>
     </row>
-    <row r="620">
+    <row r="620" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E620" s="11"/>
     </row>
-    <row r="621">
+    <row r="621" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E621" s="11"/>
     </row>
-    <row r="622">
+    <row r="622" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E622" s="11"/>
     </row>
-    <row r="623">
+    <row r="623" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E623" s="11"/>
     </row>
-    <row r="624">
+    <row r="624" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E624" s="11"/>
     </row>
-    <row r="625">
+    <row r="625" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E625" s="11"/>
     </row>
-    <row r="626">
+    <row r="626" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E626" s="11"/>
     </row>
-    <row r="627">
+    <row r="627" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E627" s="11"/>
     </row>
-    <row r="628">
+    <row r="628" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E628" s="11"/>
     </row>
-    <row r="629">
+    <row r="629" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E629" s="11"/>
     </row>
-    <row r="630">
+    <row r="630" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E630" s="11"/>
     </row>
-    <row r="631">
+    <row r="631" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E631" s="11"/>
     </row>
-    <row r="632">
+    <row r="632" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E632" s="11"/>
     </row>
-    <row r="633">
+    <row r="633" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E633" s="11"/>
     </row>
-    <row r="634">
+    <row r="634" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E634" s="11"/>
     </row>
-    <row r="635">
+    <row r="635" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E635" s="11"/>
     </row>
-    <row r="636">
+    <row r="636" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E636" s="11"/>
     </row>
-    <row r="637">
+    <row r="637" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E637" s="11"/>
     </row>
-    <row r="638">
+    <row r="638" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E638" s="11"/>
     </row>
-    <row r="639">
+    <row r="639" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E639" s="11"/>
     </row>
-    <row r="640">
+    <row r="640" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E640" s="11"/>
     </row>
-    <row r="641">
+    <row r="641" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E641" s="11"/>
     </row>
-    <row r="642">
+    <row r="642" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E642" s="11"/>
     </row>
-    <row r="643">
+    <row r="643" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E643" s="11"/>
     </row>
-    <row r="644">
+    <row r="644" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E644" s="11"/>
     </row>
-    <row r="645">
+    <row r="645" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E645" s="11"/>
     </row>
-    <row r="646">
+    <row r="646" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E646" s="11"/>
     </row>
-    <row r="647">
+    <row r="647" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E647" s="11"/>
     </row>
-    <row r="648">
+    <row r="648" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E648" s="11"/>
     </row>
-    <row r="649">
+    <row r="649" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E649" s="11"/>
     </row>
-    <row r="650">
+    <row r="650" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E650" s="11"/>
     </row>
-    <row r="651">
+    <row r="651" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E651" s="11"/>
     </row>
-    <row r="652">
+    <row r="652" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E652" s="11"/>
     </row>
-    <row r="653">
+    <row r="653" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E653" s="11"/>
     </row>
-    <row r="654">
+    <row r="654" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E654" s="11"/>
     </row>
-    <row r="655">
+    <row r="655" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E655" s="11"/>
     </row>
-    <row r="656">
+    <row r="656" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E656" s="11"/>
     </row>
-    <row r="657">
+    <row r="657" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E657" s="11"/>
     </row>
-    <row r="658">
+    <row r="658" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E658" s="11"/>
     </row>
-    <row r="659">
+    <row r="659" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E659" s="11"/>
     </row>
-    <row r="660">
+    <row r="660" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E660" s="11"/>
     </row>
-    <row r="661">
+    <row r="661" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E661" s="11"/>
     </row>
-    <row r="662">
+    <row r="662" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E662" s="11"/>
     </row>
-    <row r="663">
+    <row r="663" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E663" s="11"/>
     </row>
-    <row r="664">
+    <row r="664" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E664" s="11"/>
     </row>
-    <row r="665">
+    <row r="665" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E665" s="11"/>
     </row>
-    <row r="666">
+    <row r="666" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E666" s="11"/>
     </row>
-    <row r="667">
+    <row r="667" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E667" s="11"/>
     </row>
-    <row r="668">
+    <row r="668" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E668" s="11"/>
     </row>
-    <row r="669">
+    <row r="669" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E669" s="11"/>
     </row>
-    <row r="670">
+    <row r="670" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E670" s="11"/>
     </row>
-    <row r="671">
+    <row r="671" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E671" s="11"/>
     </row>
-    <row r="672">
+    <row r="672" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E672" s="11"/>
     </row>
-    <row r="673">
+    <row r="673" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E673" s="11"/>
     </row>
-    <row r="674">
+    <row r="674" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E674" s="11"/>
     </row>
-    <row r="675">
+    <row r="675" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E675" s="11"/>
     </row>
-    <row r="676">
+    <row r="676" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E676" s="11"/>
     </row>
-    <row r="677">
+    <row r="677" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E677" s="11"/>
     </row>
-    <row r="678">
+    <row r="678" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E678" s="11"/>
     </row>
-    <row r="679">
+    <row r="679" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E679" s="11"/>
     </row>
-    <row r="680">
+    <row r="680" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E680" s="11"/>
     </row>
-    <row r="681">
+    <row r="681" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E681" s="11"/>
     </row>
-    <row r="682">
+    <row r="682" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E682" s="11"/>
     </row>
-    <row r="683">
+    <row r="683" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E683" s="11"/>
     </row>
-    <row r="684">
+    <row r="684" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E684" s="11"/>
     </row>
-    <row r="685">
+    <row r="685" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E685" s="11"/>
     </row>
-    <row r="686">
+    <row r="686" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E686" s="11"/>
     </row>
-    <row r="687">
+    <row r="687" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E687" s="11"/>
     </row>
-    <row r="688">
+    <row r="688" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E688" s="11"/>
     </row>
-    <row r="689">
+    <row r="689" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E689" s="11"/>
     </row>
-    <row r="690">
+    <row r="690" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E690" s="11"/>
     </row>
-    <row r="691">
+    <row r="691" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E691" s="11"/>
     </row>
-    <row r="692">
+    <row r="692" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E692" s="11"/>
     </row>
-    <row r="693">
+    <row r="693" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E693" s="11"/>
     </row>
-    <row r="694">
+    <row r="694" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E694" s="11"/>
     </row>
-    <row r="695">
+    <row r="695" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E695" s="11"/>
     </row>
-    <row r="696">
+    <row r="696" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E696" s="11"/>
     </row>
-    <row r="697">
+    <row r="697" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E697" s="11"/>
     </row>
-    <row r="698">
+    <row r="698" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E698" s="11"/>
     </row>
-    <row r="699">
+    <row r="699" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E699" s="11"/>
     </row>
-    <row r="700">
+    <row r="700" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E700" s="11"/>
     </row>
-    <row r="701">
+    <row r="701" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E701" s="11"/>
     </row>
-    <row r="702">
+    <row r="702" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E702" s="11"/>
     </row>
-    <row r="703">
+    <row r="703" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E703" s="11"/>
     </row>
-    <row r="704">
+    <row r="704" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E704" s="11"/>
     </row>
-    <row r="705">
+    <row r="705" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E705" s="11"/>
     </row>
-    <row r="706">
+    <row r="706" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E706" s="11"/>
     </row>
-    <row r="707">
+    <row r="707" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E707" s="11"/>
     </row>
-    <row r="708">
+    <row r="708" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E708" s="11"/>
     </row>
-    <row r="709">
+    <row r="709" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E709" s="11"/>
     </row>
-    <row r="710">
+    <row r="710" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E710" s="11"/>
     </row>
-    <row r="711">
+    <row r="711" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E711" s="11"/>
     </row>
-    <row r="712">
+    <row r="712" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E712" s="11"/>
     </row>
-    <row r="713">
+    <row r="713" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E713" s="11"/>
     </row>
-    <row r="714">
+    <row r="714" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E714" s="11"/>
     </row>
-    <row r="715">
+    <row r="715" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E715" s="11"/>
     </row>
-    <row r="716">
+    <row r="716" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E716" s="11"/>
     </row>
-    <row r="717">
+    <row r="717" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E717" s="11"/>
     </row>
-    <row r="718">
+    <row r="718" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E718" s="11"/>
     </row>
-    <row r="719">
+    <row r="719" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E719" s="11"/>
     </row>
-    <row r="720">
+    <row r="720" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E720" s="11"/>
     </row>
-    <row r="721">
+    <row r="721" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E721" s="11"/>
     </row>
-    <row r="722">
+    <row r="722" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E722" s="11"/>
     </row>
-    <row r="723">
+    <row r="723" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E723" s="11"/>
     </row>
-    <row r="724">
+    <row r="724" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E724" s="11"/>
     </row>
-    <row r="725">
+    <row r="725" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E725" s="11"/>
     </row>
-    <row r="726">
+    <row r="726" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E726" s="11"/>
     </row>
-    <row r="727">
+    <row r="727" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E727" s="11"/>
     </row>
-    <row r="728">
+    <row r="728" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E728" s="11"/>
     </row>
-    <row r="729">
+    <row r="729" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E729" s="11"/>
     </row>
-    <row r="730">
+    <row r="730" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E730" s="11"/>
     </row>
-    <row r="731">
+    <row r="731" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E731" s="11"/>
     </row>
-    <row r="732">
+    <row r="732" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E732" s="11"/>
     </row>
-    <row r="733">
+    <row r="733" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E733" s="11"/>
     </row>
-    <row r="734">
+    <row r="734" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E734" s="11"/>
     </row>
-    <row r="735">
+    <row r="735" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E735" s="11"/>
     </row>
-    <row r="736">
+    <row r="736" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E736" s="11"/>
     </row>
-    <row r="737">
+    <row r="737" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E737" s="11"/>
     </row>
-    <row r="738">
+    <row r="738" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E738" s="11"/>
     </row>
-    <row r="739">
+    <row r="739" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E739" s="11"/>
     </row>
-    <row r="740">
+    <row r="740" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E740" s="11"/>
     </row>
-    <row r="741">
+    <row r="741" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E741" s="11"/>
     </row>
-    <row r="742">
+    <row r="742" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E742" s="11"/>
     </row>
-    <row r="743">
+    <row r="743" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E743" s="11"/>
     </row>
-    <row r="744">
+    <row r="744" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E744" s="11"/>
     </row>
-    <row r="745">
+    <row r="745" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E745" s="11"/>
     </row>
-    <row r="746">
+    <row r="746" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E746" s="11"/>
     </row>
-    <row r="747">
+    <row r="747" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E747" s="11"/>
     </row>
-    <row r="748">
+    <row r="748" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E748" s="11"/>
     </row>
-    <row r="749">
+    <row r="749" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E749" s="11"/>
     </row>
-    <row r="750">
+    <row r="750" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E750" s="11"/>
     </row>
-    <row r="751">
+    <row r="751" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E751" s="11"/>
     </row>
-    <row r="752">
+    <row r="752" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E752" s="11"/>
     </row>
-    <row r="753">
+    <row r="753" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E753" s="11"/>
     </row>
-    <row r="754">
+    <row r="754" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E754" s="11"/>
     </row>
-    <row r="755">
+    <row r="755" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E755" s="11"/>
     </row>
-    <row r="756">
+    <row r="756" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E756" s="11"/>
     </row>
-    <row r="757">
+    <row r="757" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E757" s="11"/>
     </row>
-    <row r="758">
+    <row r="758" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E758" s="11"/>
     </row>
-    <row r="759">
+    <row r="759" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E759" s="11"/>
     </row>
-    <row r="760">
+    <row r="760" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E760" s="11"/>
     </row>
-    <row r="761">
+    <row r="761" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E761" s="11"/>
     </row>
-    <row r="762">
+    <row r="762" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E762" s="11"/>
     </row>
-    <row r="763">
+    <row r="763" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E763" s="11"/>
     </row>
-    <row r="764">
+    <row r="764" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E764" s="11"/>
     </row>
-    <row r="765">
+    <row r="765" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E765" s="11"/>
     </row>
-    <row r="766">
+    <row r="766" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E766" s="11"/>
     </row>
-    <row r="767">
+    <row r="767" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E767" s="11"/>
     </row>
-    <row r="768">
+    <row r="768" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E768" s="11"/>
     </row>
-    <row r="769">
+    <row r="769" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E769" s="11"/>
     </row>
-    <row r="770">
+    <row r="770" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E770" s="11"/>
     </row>
-    <row r="771">
+    <row r="771" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E771" s="11"/>
     </row>
-    <row r="772">
+    <row r="772" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E772" s="11"/>
     </row>
-    <row r="773">
+    <row r="773" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E773" s="11"/>
     </row>
-    <row r="774">
+    <row r="774" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E774" s="11"/>
     </row>
-    <row r="775">
+    <row r="775" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E775" s="11"/>
     </row>
-    <row r="776">
+    <row r="776" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E776" s="11"/>
     </row>
-    <row r="777">
+    <row r="777" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E777" s="11"/>
     </row>
-    <row r="778">
+    <row r="778" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E778" s="11"/>
     </row>
-    <row r="779">
+    <row r="779" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E779" s="11"/>
     </row>
-    <row r="780">
+    <row r="780" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E780" s="11"/>
     </row>
-    <row r="781">
+    <row r="781" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E781" s="11"/>
     </row>
-    <row r="782">
+    <row r="782" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E782" s="11"/>
     </row>
-    <row r="783">
+    <row r="783" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E783" s="11"/>
     </row>
-    <row r="784">
+    <row r="784" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E784" s="11"/>
     </row>
-    <row r="785">
+    <row r="785" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E785" s="11"/>
     </row>
-    <row r="786">
+    <row r="786" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E786" s="11"/>
     </row>
-    <row r="787">
+    <row r="787" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E787" s="11"/>
     </row>
-    <row r="788">
+    <row r="788" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E788" s="11"/>
     </row>
-    <row r="789">
+    <row r="789" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E789" s="11"/>
     </row>
-    <row r="790">
+    <row r="790" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E790" s="11"/>
     </row>
-    <row r="791">
+    <row r="791" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E791" s="11"/>
     </row>
-    <row r="792">
+    <row r="792" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E792" s="11"/>
     </row>
-    <row r="793">
+    <row r="793" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E793" s="11"/>
     </row>
-    <row r="794">
+    <row r="794" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E794" s="11"/>
     </row>
-    <row r="795">
+    <row r="795" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E795" s="11"/>
     </row>
-    <row r="796">
+    <row r="796" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E796" s="11"/>
     </row>
-    <row r="797">
+    <row r="797" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E797" s="11"/>
     </row>
-    <row r="798">
+    <row r="798" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E798" s="11"/>
     </row>
-    <row r="799">
+    <row r="799" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E799" s="11"/>
     </row>
-    <row r="800">
+    <row r="800" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E800" s="11"/>
     </row>
-    <row r="801">
+    <row r="801" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E801" s="11"/>
     </row>
-    <row r="802">
+    <row r="802" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E802" s="11"/>
     </row>
-    <row r="803">
+    <row r="803" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E803" s="11"/>
     </row>
-    <row r="804">
+    <row r="804" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E804" s="11"/>
     </row>
-    <row r="805">
+    <row r="805" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E805" s="11"/>
     </row>
-    <row r="806">
+    <row r="806" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E806" s="11"/>
     </row>
-    <row r="807">
+    <row r="807" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E807" s="11"/>
     </row>
-    <row r="808">
+    <row r="808" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E808" s="11"/>
     </row>
-    <row r="809">
+    <row r="809" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E809" s="11"/>
     </row>
-    <row r="810">
+    <row r="810" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E810" s="11"/>
     </row>
-    <row r="811">
+    <row r="811" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E811" s="11"/>
     </row>
-    <row r="812">
+    <row r="812" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E812" s="11"/>
     </row>
-    <row r="813">
+    <row r="813" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E813" s="11"/>
     </row>
-    <row r="814">
+    <row r="814" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E814" s="11"/>
     </row>
-    <row r="815">
+    <row r="815" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E815" s="11"/>
     </row>
-    <row r="816">
+    <row r="816" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E816" s="11"/>
     </row>
-    <row r="817">
+    <row r="817" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E817" s="11"/>
     </row>
-    <row r="818">
+    <row r="818" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E818" s="11"/>
     </row>
-    <row r="819">
+    <row r="819" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E819" s="11"/>
     </row>
-    <row r="820">
+    <row r="820" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E820" s="11"/>
     </row>
-    <row r="821">
+    <row r="821" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E821" s="11"/>
     </row>
-    <row r="822">
+    <row r="822" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E822" s="11"/>
     </row>
-    <row r="823">
+    <row r="823" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E823" s="11"/>
     </row>
-    <row r="824">
+    <row r="824" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E824" s="11"/>
     </row>
-    <row r="825">
+    <row r="825" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E825" s="11"/>
     </row>
-    <row r="826">
+    <row r="826" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E826" s="11"/>
     </row>
-    <row r="827">
+    <row r="827" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E827" s="11"/>
     </row>
-    <row r="828">
+    <row r="828" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E828" s="11"/>
     </row>
-    <row r="829">
+    <row r="829" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E829" s="11"/>
     </row>
-    <row r="830">
+    <row r="830" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E830" s="11"/>
     </row>
-    <row r="831">
+    <row r="831" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E831" s="11"/>
     </row>
-    <row r="832">
+    <row r="832" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E832" s="11"/>
     </row>
-    <row r="833">
+    <row r="833" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E833" s="11"/>
     </row>
-    <row r="834">
+    <row r="834" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E834" s="11"/>
     </row>
-    <row r="835">
+    <row r="835" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E835" s="11"/>
     </row>
-    <row r="836">
+    <row r="836" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E836" s="11"/>
     </row>
-    <row r="837">
+    <row r="837" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E837" s="11"/>
     </row>
-    <row r="838">
+    <row r="838" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E838" s="11"/>
     </row>
-    <row r="839">
+    <row r="839" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E839" s="11"/>
     </row>
-    <row r="840">
+    <row r="840" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E840" s="11"/>
     </row>
-    <row r="841">
+    <row r="841" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E841" s="11"/>
     </row>
-    <row r="842">
+    <row r="842" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E842" s="11"/>
     </row>
-    <row r="843">
+    <row r="843" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E843" s="11"/>
     </row>
-    <row r="844">
+    <row r="844" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E844" s="11"/>
     </row>
-    <row r="845">
+    <row r="845" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E845" s="11"/>
     </row>
-    <row r="846">
+    <row r="846" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E846" s="11"/>
     </row>
-    <row r="847">
+    <row r="847" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E847" s="11"/>
     </row>
-    <row r="848">
+    <row r="848" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E848" s="11"/>
     </row>
-    <row r="849">
+    <row r="849" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E849" s="11"/>
     </row>
-    <row r="850">
+    <row r="850" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E850" s="11"/>
     </row>
-    <row r="851">
+    <row r="851" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E851" s="11"/>
     </row>
-    <row r="852">
+    <row r="852" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E852" s="11"/>
     </row>
-    <row r="853">
+    <row r="853" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E853" s="11"/>
     </row>
-    <row r="854">
+    <row r="854" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E854" s="11"/>
     </row>
-    <row r="855">
+    <row r="855" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E855" s="11"/>
     </row>
-    <row r="856">
+    <row r="856" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E856" s="11"/>
     </row>
-    <row r="857">
+    <row r="857" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E857" s="11"/>
     </row>
-    <row r="858">
+    <row r="858" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E858" s="11"/>
     </row>
-    <row r="859">
+    <row r="859" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E859" s="11"/>
     </row>
-    <row r="860">
+    <row r="860" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E860" s="11"/>
     </row>
-    <row r="861">
+    <row r="861" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E861" s="11"/>
     </row>
-    <row r="862">
+    <row r="862" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E862" s="11"/>
     </row>
-    <row r="863">
+    <row r="863" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E863" s="11"/>
     </row>
-    <row r="864">
+    <row r="864" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E864" s="11"/>
     </row>
-    <row r="865">
+    <row r="865" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E865" s="11"/>
     </row>
-    <row r="866">
+    <row r="866" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E866" s="11"/>
     </row>
-    <row r="867">
+    <row r="867" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E867" s="11"/>
     </row>
-    <row r="868">
+    <row r="868" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E868" s="11"/>
     </row>
-    <row r="869">
+    <row r="869" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E869" s="11"/>
     </row>
-    <row r="870">
+    <row r="870" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E870" s="11"/>
     </row>
-    <row r="871">
+    <row r="871" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E871" s="11"/>
     </row>
-    <row r="872">
+    <row r="872" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E872" s="11"/>
     </row>
-    <row r="873">
+    <row r="873" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E873" s="11"/>
     </row>
-    <row r="874">
+    <row r="874" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E874" s="11"/>
     </row>
-    <row r="875">
+    <row r="875" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E875" s="11"/>
     </row>
-    <row r="876">
+    <row r="876" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E876" s="11"/>
     </row>
-    <row r="877">
+    <row r="877" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E877" s="11"/>
     </row>
-    <row r="878">
+    <row r="878" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E878" s="11"/>
     </row>
-    <row r="879">
+    <row r="879" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E879" s="11"/>
     </row>
-    <row r="880">
+    <row r="880" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E880" s="11"/>
     </row>
-    <row r="881">
+    <row r="881" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E881" s="11"/>
     </row>
-    <row r="882">
+    <row r="882" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E882" s="11"/>
     </row>
-    <row r="883">
+    <row r="883" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E883" s="11"/>
     </row>
-    <row r="884">
+    <row r="884" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E884" s="11"/>
     </row>
-    <row r="885">
+    <row r="885" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E885" s="11"/>
     </row>
-    <row r="886">
+    <row r="886" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E886" s="11"/>
     </row>
-    <row r="887">
+    <row r="887" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E887" s="11"/>
     </row>
-    <row r="888">
+    <row r="888" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E888" s="11"/>
     </row>
-    <row r="889">
+    <row r="889" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E889" s="11"/>
     </row>
-    <row r="890">
+    <row r="890" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E890" s="11"/>
     </row>
-    <row r="891">
+    <row r="891" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E891" s="11"/>
     </row>
-    <row r="892">
+    <row r="892" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E892" s="11"/>
     </row>
-    <row r="893">
+    <row r="893" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E893" s="11"/>
     </row>
-    <row r="894">
+    <row r="894" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E894" s="11"/>
     </row>
-    <row r="895">
+    <row r="895" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E895" s="11"/>
     </row>
-    <row r="896">
+    <row r="896" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E896" s="11"/>
     </row>
-    <row r="897">
+    <row r="897" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E897" s="11"/>
     </row>
-    <row r="898">
+    <row r="898" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E898" s="11"/>
     </row>
-    <row r="899">
+    <row r="899" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E899" s="11"/>
     </row>
-    <row r="900">
+    <row r="900" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E900" s="11"/>
     </row>
-    <row r="901">
+    <row r="901" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E901" s="11"/>
     </row>
-    <row r="902">
+    <row r="902" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E902" s="11"/>
     </row>
-    <row r="903">
+    <row r="903" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E903" s="11"/>
     </row>
-    <row r="904">
+    <row r="904" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E904" s="11"/>
     </row>
-    <row r="905">
+    <row r="905" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E905" s="11"/>
     </row>
-    <row r="906">
+    <row r="906" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E906" s="11"/>
     </row>
-    <row r="907">
+    <row r="907" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E907" s="11"/>
     </row>
-    <row r="908">
+    <row r="908" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E908" s="11"/>
     </row>
-    <row r="909">
+    <row r="909" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E909" s="11"/>
     </row>
-    <row r="910">
+    <row r="910" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E910" s="11"/>
     </row>
-    <row r="911">
+    <row r="911" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E911" s="11"/>
     </row>
-    <row r="912">
+    <row r="912" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E912" s="11"/>
     </row>
-    <row r="913">
+    <row r="913" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E913" s="11"/>
     </row>
-    <row r="914">
+    <row r="914" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E914" s="11"/>
     </row>
-    <row r="915">
+    <row r="915" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E915" s="11"/>
     </row>
-    <row r="916">
+    <row r="916" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E916" s="11"/>
     </row>
-    <row r="917">
+    <row r="917" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E917" s="11"/>
     </row>
-    <row r="918">
+    <row r="918" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E918" s="11"/>
     </row>
-    <row r="919">
+    <row r="919" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E919" s="11"/>
     </row>
-    <row r="920">
+    <row r="920" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E920" s="11"/>
     </row>
-    <row r="921">
+    <row r="921" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E921" s="11"/>
     </row>
-    <row r="922">
+    <row r="922" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E922" s="11"/>
     </row>
-    <row r="923">
+    <row r="923" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E923" s="11"/>
     </row>
-    <row r="924">
+    <row r="924" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E924" s="11"/>
     </row>
-    <row r="925">
+    <row r="925" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E925" s="11"/>
     </row>
-    <row r="926">
+    <row r="926" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E926" s="11"/>
     </row>
-    <row r="927">
+    <row r="927" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E927" s="11"/>
     </row>
-    <row r="928">
+    <row r="928" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E928" s="11"/>
     </row>
-    <row r="929">
+    <row r="929" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E929" s="11"/>
     </row>
-    <row r="930">
+    <row r="930" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E930" s="11"/>
     </row>
-    <row r="931">
+    <row r="931" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E931" s="11"/>
     </row>
-    <row r="932">
+    <row r="932" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E932" s="11"/>
     </row>
-    <row r="933">
+    <row r="933" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E933" s="11"/>
     </row>
-    <row r="934">
+    <row r="934" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E934" s="11"/>
     </row>
-    <row r="935">
+    <row r="935" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E935" s="11"/>
     </row>
-    <row r="936">
+    <row r="936" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E936" s="11"/>
     </row>
-    <row r="937">
+    <row r="937" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E937" s="11"/>
     </row>
-    <row r="938">
+    <row r="938" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E938" s="11"/>
     </row>
-    <row r="939">
+    <row r="939" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E939" s="11"/>
     </row>
-    <row r="940">
+    <row r="940" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E940" s="11"/>
     </row>
-    <row r="941">
+    <row r="941" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E941" s="11"/>
     </row>
-    <row r="942">
+    <row r="942" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E942" s="11"/>
     </row>
-    <row r="943">
+    <row r="943" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E943" s="11"/>
     </row>
-    <row r="944">
+    <row r="944" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E944" s="11"/>
     </row>
-    <row r="945">
+    <row r="945" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E945" s="11"/>
     </row>
-    <row r="946">
+    <row r="946" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E946" s="11"/>
     </row>
-    <row r="947">
+    <row r="947" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E947" s="11"/>
     </row>
-    <row r="948">
+    <row r="948" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E948" s="11"/>
     </row>
-    <row r="949">
+    <row r="949" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E949" s="11"/>
     </row>
-    <row r="950">
+    <row r="950" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E950" s="11"/>
     </row>
-    <row r="951">
+    <row r="951" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E951" s="11"/>
     </row>
-    <row r="952">
+    <row r="952" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E952" s="11"/>
     </row>
-    <row r="953">
+    <row r="953" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E953" s="11"/>
     </row>
-    <row r="954">
+    <row r="954" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E954" s="11"/>
     </row>
-    <row r="955">
+    <row r="955" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E955" s="11"/>
     </row>
-    <row r="956">
+    <row r="956" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E956" s="11"/>
     </row>
-    <row r="957">
+    <row r="957" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E957" s="11"/>
     </row>
-    <row r="958">
+    <row r="958" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E958" s="11"/>
     </row>
-    <row r="959">
+    <row r="959" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E959" s="11"/>
     </row>
-    <row r="960">
+    <row r="960" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E960" s="11"/>
     </row>
-    <row r="961">
+    <row r="961" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E961" s="11"/>
     </row>
-    <row r="962">
+    <row r="962" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E962" s="11"/>
     </row>
-    <row r="963">
+    <row r="963" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E963" s="11"/>
     </row>
-    <row r="964">
+    <row r="964" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E964" s="11"/>
     </row>
-    <row r="965">
+    <row r="965" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E965" s="11"/>
     </row>
-    <row r="966">
+    <row r="966" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E966" s="11"/>
     </row>
-    <row r="967">
+    <row r="967" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E967" s="11"/>
     </row>
-    <row r="968">
+    <row r="968" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E968" s="11"/>
     </row>
-    <row r="969">
+    <row r="969" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E969" s="11"/>
     </row>
-    <row r="970">
+    <row r="970" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E970" s="11"/>
     </row>
-    <row r="971">
+    <row r="971" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E971" s="11"/>
     </row>
-    <row r="972">
+    <row r="972" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E972" s="11"/>
     </row>
-    <row r="973">
+    <row r="973" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E973" s="11"/>
     </row>
-    <row r="974">
+    <row r="974" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E974" s="11"/>
     </row>
-    <row r="975">
+    <row r="975" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E975" s="11"/>
     </row>
-    <row r="976">
+    <row r="976" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E976" s="11"/>
     </row>
-    <row r="977">
+    <row r="977" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E977" s="11"/>
     </row>
-    <row r="978">
+    <row r="978" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E978" s="11"/>
     </row>
-    <row r="979">
+    <row r="979" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E979" s="11"/>
     </row>
-    <row r="980">
+    <row r="980" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E980" s="11"/>
     </row>
-    <row r="981">
+    <row r="981" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E981" s="11"/>
     </row>
-    <row r="982">
+    <row r="982" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E982" s="11"/>
     </row>
-    <row r="983">
+    <row r="983" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E983" s="11"/>
     </row>
-    <row r="984">
+    <row r="984" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E984" s="11"/>
     </row>
-    <row r="985">
+    <row r="985" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E985" s="11"/>
     </row>
-    <row r="986">
+    <row r="986" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E986" s="11"/>
     </row>
-    <row r="987">
+    <row r="987" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E987" s="11"/>
     </row>
-    <row r="988">
+    <row r="988" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E988" s="11"/>
     </row>
-    <row r="989">
+    <row r="989" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E989" s="11"/>
     </row>
-    <row r="990">
+    <row r="990" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E990" s="11"/>
     </row>
-    <row r="991">
+    <row r="991" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E991" s="11"/>
     </row>
-    <row r="992">
+    <row r="992" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E992" s="11"/>
     </row>
-    <row r="993">
+    <row r="993" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E993" s="11"/>
     </row>
-    <row r="994">
+    <row r="994" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E994" s="11"/>
     </row>
-    <row r="995">
+    <row r="995" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E995" s="11"/>
     </row>
-    <row r="996">
+    <row r="996" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E996" s="11"/>
     </row>
-    <row r="997">
+    <row r="997" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E997" s="11"/>
     </row>
-    <row r="998">
+    <row r="998" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E998" s="11"/>
     </row>
-    <row r="999">
+    <row r="999" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E999" s="11"/>
     </row>
-    <row r="1000">
+    <row r="1000" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E1000" s="11"/>
     </row>
-    <row r="1001">
+    <row r="1001" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E1001" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>